<commit_message>
Refactor all caps code
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_all_caps.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_all_caps.xlsx
@@ -13,14 +13,14 @@
     <sheet name="2022" sheetId="4" r:id="rId4"/>
     <sheet name="2023" sheetId="5" r:id="rId5"/>
     <sheet name="2024" sheetId="6" r:id="rId6"/>
-    <sheet name="Summary" sheetId="7" r:id="rId7"/>
+    <sheet name="Proportion Summary" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -28,49 +28,22 @@
     <t>originalBodyText</t>
   </si>
   <si>
-    <t>text_length</t>
+    <t>originalTextType</t>
+  </si>
+  <si>
+    <t>proportion_upper_to_alpha_tokens</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_944914</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_58814</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_888712</t>
   </si>
   <si>
     <t>Politifact_Mostly False_Press release_41803</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_888712</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_58814</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_944914</t>
-  </si>
-  <si>
-    <t>Madison... Assembly Republican veterans are speaking out against a proposal in Governor Tony Evers’ budget that would reduce tuition for non U.S. citizens. Under the Evers proposal, college applicants in the country illegally would pay substantially reduced in-state tuition if they’ve attended a Wisconsin high school and been “present” in the state for three years. In contrast, veterans in the state must prove not only residency of five years, but prove military service and maintain their grades in order to receive tuition benefits.
-“This is a stunning display of the displaced priorities Governor Evers used to develop his budget,” said Rep. Ken Skowronski (R-Franklin). “Veterans who have served our nation are forced to meet a much higher standard to get the tuition remission they earned through sacrifice than the governor asks from illegal immigrants.”
-The Republican representatives are asking the members of the Joint Committee on Finance to remove the item from the budget. The tuition break for each illegal immigrant could run tens of thousands of dollars, much more than what veterans receive in the tuition remission program.
-“Governor Evers’s proposal shows how out of touch he is with Wisconsin’s veterans,” said Rep. Jim Ott (R-Mequon). “Of course, it should be taken out of the budget.”
-“Governor Evers has misplaced priorities if he thinks it’s acceptable that undocumented immigrants should have an easier path to in-state tuition than our veterans,” said Rep. Jesse James (R-Altoona). “It’s frankly quite disgusting and a disservice to those that have served and defended this country’s freedoms, freedoms that make it possible for the Wisconsin Idea to exist. I urge the Joint Finance Committee to remove this from the budget.”
-Under state statute, the Wisconsin veteran remission program requires veterans to prove Wisconsin residency at time of entry into service or for five consecutive years as well as proving qualifying service and maintaining a C average. Some veterans who serve Wisconsin still would not meet the residency standard and would be ineligible for the tuition program.
-“The Evers plan says three years for illegal immigrants to get special tuition benefits, but five years for veterans,” said Rep. Tony Kurtz (R-Wonewoc). “We are talking about people who fought for our freedom and deserve our respect and gratitude.”</t>
-  </si>
-  <si>
-    <t>Meets with Border Trade Alliance, Rio Grande Valley Partnership, highlights crisis at Texas-Mexico border on Ben Shapiro Show
-HOUSTON, Texas - U.S. Sen. Ted Cruz (R-Texas) this week held meetings in his Washington, D.C. Senate office with members of the Border Trade Alliance and the Rio Grande Valley Partnership. In those meetings, Sen. Cruz participated in a dialogue with the members, and discussed his views regarding trade and immigration, among other issues facing the Texas-Mexico border.
-During his meeting with the Border Trade Alliance, Sen. Cruz highlighted the over 144,000 apprehensions on the Texas-Mexico border, which continue to overwhelm infrastructure and border communities.
-"The Texas border is a wonderful place," Sen. Cruz said to the Border Trade Alliance. "Unfortunately right now, the border is a flashpoint for enormous political disagreement. On border security, what we are seeing is a crisis. As you know, we apprehended over 144,000 people in a single month. That is a pace, which if it continues for 12 months, would put us on a pace for nearly two million apprehensions on the border. That exceeds what we can handle. And I've heard from a number of you in this room about how the volume of illegal crossings is now overwhelming infrastructure, overwhelming the ability of the communities to absorb that much population coming in."
-In his meeting with the Rio Grande Valley Partnership, Sen. Cruz reiterated his commitment to devoting the resources necessary for securing the border.
-"I have heard from leaders in the Valley, I have heard from leaders up and down the border that it is swamping the capacity of the communities to deal with that volume of people coming," Sen. Cruz said to the Rio Grande Valley Partnership. "That is exceeds the infrastructure capacity. And I can tell you on my end that I am pressing hard for us to devote the resources necessary to deal with the incredible influx of people coming illegally, but also to close the loopholes that Congress has put in place."
-Sen. Cruz also addressed the issue of trade with the groups, noting that the border is a "thriving example" of international trade.
-"The single most frequent concern I hear from Texas business leaders is trade," Sen. Cruz said to the Border Trade Alliance. "I know there is a lot of anxiety in this room over trade and I understand that; you are not crazy to be anxious about it. Within the Trump administration, there are divided voices. Some voices within the administration want to tear down the barriers of our trading partners, to letting our goods and services into their markets and want to increase international trade. Other voices in the administration want to erect barriers into our own markets and want to decrease international trade. Between those two, I am emphatically in the camp of the former and not the latter. I believe in international trade. Texas does well, Texas farmers, ranchers, manufacturers, and small businesses, we do well if our markets are open and the border is a thriving example of that. I have had the great pleasure of touring factories and plants and businesses all up and down the border and it is incredible, the opportunity that we are seeing, flourishing on the border through doing trade with Mexico and more broadly with the world."
-When asked about the ongoing crisis at the border on the Ben Shapiro Show, Sen. Cruz urged his colleagues in Congress to provide the resources necessary to secure the border and build the wall. Listen to the full interview here.
-"We are seeing an absolute crisis on the border," Sen. Cruz said. "My home state of Texas, of the 2,000 miles of border the United States has with Mexico, 1,200 of those miles are in Texas. And we are seeing the crisis, you know when I'm down at the border, I spend a lot of time at the border, when I'm down at the border and the Rio Grande Valley, or all along the border, local officials there say they are being overwhelmed, and these are elected Democrats on the border but they are saying the volume of illegal immigration is so overwhelming right now.
-"The position of congressional Democrats is essentially they are telling everyone ‘go jump in a lake,'" Sen. Cruz continued. "The president, the administration has asked for a supplemental funding bill of $4.5 billion to provide the resources to deal with this crisis at the border and to date, congressional Democrats have said ‘hell no,' they are not willing to do anything. I hope that they change. That is really a heartless position, and my understanding is next week, the Senate is going to vote on this, so we will see where Senate Democrats line up. But right now, they are telling those children who are coming across the border that they are not willing to provide any resources that those kids, those families need -- that we need to secure the border and stop this crisis."</t>
-  </si>
-  <si>
-    <t>Trump promised to bring manufacturing jobs back to Pennsylvania and Wisconsin — that hasn’t happened. Instead, Pennsylvania and Wisconsin have lost the most manufacturing jobs in the past year.
-PROMISE MADE: Trump promised to bring manufacturing jobs back to Pennsylvania and Wisconsin.
-Trump in Pennsylvania: “We’re going to bring back our manufacturing, we’re going to bring back our jobs that formed the backbone of the American middle class and our country as a whole.” [Valley Forge PA, 11/1/16]
-Trump in Wisconsin: “I just had this written out and this is about Wisconsin trade facts. Twenty percent of manufacturing jobs have left since 2000. Nobody knows that. We’ll get you a job. We’ll get you a lot of jobs. We’re bringing our jobs back from China. We’re bringing out jobs back from Mexico. We’re going to stop people from moving to Mexico.” [Racine WI, 4/2/16]
-PROMISE BROKEN: Pennsylvania and Wisconsin have lost the most manufacturing jobs in the past year.
-Bloomberg: “The two swing states lost the most manufacturing jobs in the past 12 months, bucking the national trend. In Pennsylvania, home to steel mills, the number of factory positions fell by about 8,000 and in Wisconsin the loss was just over 5,000, according to regional data from the Labor Department Friday.”</t>
   </si>
   <si>
     <t>In September, I attended a CNN town hall on the climate crisis. That night, Bren Smith, an ocean farmer from Connecticut, asked me if I would support a Blue New Deal to restore our oceans, in addition to our efforts to fight climate change on land. I said I would, and I meant it - here’s what I’ll do to rebuild our blue economy, protect and restore ocean habitat, and adapt in a climate changed world.
@@ -142,60 +115,77 @@
 Starting on day one of my presidency, I will take bold action to fight climate change. And that includes harnessing the power of our oceans to be a key part of our solution to the climate crisis. The task before us is significant, but I am confident that America is up to the challenge - both at home and around the world - to conserve and sustainably use the oceans, seas and marine resources for sustainable development. Our oceans can underpin a sustainable food system, be a source of renewable energy and defend against the worst of climate change. The future of our planet depends on a healthy ocean, and we have no more time to waste.</t>
   </si>
   <si>
+    <t>Trump promised to bring manufacturing jobs back to Pennsylvania and Wisconsin — that hasn’t happened. Instead, Pennsylvania and Wisconsin have lost the most manufacturing jobs in the past year.
+PROMISE MADE: Trump promised to bring manufacturing jobs back to Pennsylvania and Wisconsin.
+Trump in Pennsylvania: “We’re going to bring back our manufacturing, we’re going to bring back our jobs that formed the backbone of the American middle class and our country as a whole.” [Valley Forge PA, 11/1/16]
+Trump in Wisconsin: “I just had this written out and this is about Wisconsin trade facts. Twenty percent of manufacturing jobs have left since 2000. Nobody knows that. We’ll get you a job. We’ll get you a lot of jobs. We’re bringing our jobs back from China. We’re bringing out jobs back from Mexico. We’re going to stop people from moving to Mexico.” [Racine WI, 4/2/16]
+PROMISE BROKEN: Pennsylvania and Wisconsin have lost the most manufacturing jobs in the past year.
+Bloomberg: “The two swing states lost the most manufacturing jobs in the past 12 months, bucking the national trend. In Pennsylvania, home to steel mills, the number of factory positions fell by about 8,000 and in Wisconsin the loss was just over 5,000, according to regional data from the Labor Department Friday.”</t>
+  </si>
+  <si>
+    <t>Meets with Border Trade Alliance, Rio Grande Valley Partnership, highlights crisis at Texas-Mexico border on Ben Shapiro Show
+HOUSTON, Texas - U.S. Sen. Ted Cruz (R-Texas) this week held meetings in his Washington, D.C. Senate office with members of the Border Trade Alliance and the Rio Grande Valley Partnership. In those meetings, Sen. Cruz participated in a dialogue with the members, and discussed his views regarding trade and immigration, among other issues facing the Texas-Mexico border.
+During his meeting with the Border Trade Alliance, Sen. Cruz highlighted the over 144,000 apprehensions on the Texas-Mexico border, which continue to overwhelm infrastructure and border communities.
+"The Texas border is a wonderful place," Sen. Cruz said to the Border Trade Alliance. "Unfortunately right now, the border is a flashpoint for enormous political disagreement. On border security, what we are seeing is a crisis. As you know, we apprehended over 144,000 people in a single month. That is a pace, which if it continues for 12 months, would put us on a pace for nearly two million apprehensions on the border. That exceeds what we can handle. And I've heard from a number of you in this room about how the volume of illegal crossings is now overwhelming infrastructure, overwhelming the ability of the communities to absorb that much population coming in."
+In his meeting with the Rio Grande Valley Partnership, Sen. Cruz reiterated his commitment to devoting the resources necessary for securing the border.
+"I have heard from leaders in the Valley, I have heard from leaders up and down the border that it is swamping the capacity of the communities to deal with that volume of people coming," Sen. Cruz said to the Rio Grande Valley Partnership. "That is exceeds the infrastructure capacity. And I can tell you on my end that I am pressing hard for us to devote the resources necessary to deal with the incredible influx of people coming illegally, but also to close the loopholes that Congress has put in place."
+Sen. Cruz also addressed the issue of trade with the groups, noting that the border is a "thriving example" of international trade.
+"The single most frequent concern I hear from Texas business leaders is trade," Sen. Cruz said to the Border Trade Alliance. "I know there is a lot of anxiety in this room over trade and I understand that; you are not crazy to be anxious about it. Within the Trump administration, there are divided voices. Some voices within the administration want to tear down the barriers of our trading partners, to letting our goods and services into their markets and want to increase international trade. Other voices in the administration want to erect barriers into our own markets and want to decrease international trade. Between those two, I am emphatically in the camp of the former and not the latter. I believe in international trade. Texas does well, Texas farmers, ranchers, manufacturers, and small businesses, we do well if our markets are open and the border is a thriving example of that. I have had the great pleasure of touring factories and plants and businesses all up and down the border and it is incredible, the opportunity that we are seeing, flourishing on the border through doing trade with Mexico and more broadly with the world."
+When asked about the ongoing crisis at the border on the Ben Shapiro Show, Sen. Cruz urged his colleagues in Congress to provide the resources necessary to secure the border and build the wall. Listen to the full interview here.
+"We are seeing an absolute crisis on the border," Sen. Cruz said. "My home state of Texas, of the 2,000 miles of border the United States has with Mexico, 1,200 of those miles are in Texas. And we are seeing the crisis, you know when I'm down at the border, I spend a lot of time at the border, when I'm down at the border and the Rio Grande Valley, or all along the border, local officials there say they are being overwhelmed, and these are elected Democrats on the border but they are saying the volume of illegal immigration is so overwhelming right now.
+"The position of congressional Democrats is essentially they are telling everyone ‘go jump in a lake,'" Sen. Cruz continued. "The president, the administration has asked for a supplemental funding bill of $4.5 billion to provide the resources to deal with this crisis at the border and to date, congressional Democrats have said ‘hell no,' they are not willing to do anything. I hope that they change. That is really a heartless position, and my understanding is next week, the Senate is going to vote on this, so we will see where Senate Democrats line up. But right now, they are telling those children who are coming across the border that they are not willing to provide any resources that those kids, those families need -- that we need to secure the border and stop this crisis."</t>
+  </si>
+  <si>
+    <t>Madison... Assembly Republican veterans are speaking out against a proposal in Governor Tony Evers’ budget that would reduce tuition for non U.S. citizens. Under the Evers proposal, college applicants in the country illegally would pay substantially reduced in-state tuition if they’ve attended a Wisconsin high school and been “present” in the state for three years. In contrast, veterans in the state must prove not only residency of five years, but prove military service and maintain their grades in order to receive tuition benefits.
+“This is a stunning display of the displaced priorities Governor Evers used to develop his budget,” said Rep. Ken Skowronski (R-Franklin). “Veterans who have served our nation are forced to meet a much higher standard to get the tuition remission they earned through sacrifice than the governor asks from illegal immigrants.”
+The Republican representatives are asking the members of the Joint Committee on Finance to remove the item from the budget. The tuition break for each illegal immigrant could run tens of thousands of dollars, much more than what veterans receive in the tuition remission program.
+“Governor Evers’s proposal shows how out of touch he is with Wisconsin’s veterans,” said Rep. Jim Ott (R-Mequon). “Of course, it should be taken out of the budget.”
+“Governor Evers has misplaced priorities if he thinks it’s acceptable that undocumented immigrants should have an easier path to in-state tuition than our veterans,” said Rep. Jesse James (R-Altoona). “It’s frankly quite disgusting and a disservice to those that have served and defended this country’s freedoms, freedoms that make it possible for the Wisconsin Idea to exist. I urge the Joint Finance Committee to remove this from the budget.”
+Under state statute, the Wisconsin veteran remission program requires veterans to prove Wisconsin residency at time of entry into service or for five consecutive years as well as proving qualifying service and maintaining a C average. Some veterans who serve Wisconsin still would not meet the residency standard and would be ineligible for the tuition program.
+“The Evers plan says three years for illegal immigrants to get special tuition benefits, but five years for veterans,” said Rep. Tony Kurtz (R-Wonewoc). “We are talking about people who fought for our freedom and deserve our respect and gratitude.”</t>
+  </si>
+  <si>
+    <t>Press release</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_712587</t>
+  </si>
+  <si>
     <t>Politifact_FALSE_Press release_240075</t>
   </si>
   <si>
+    <t>Politifact_Mostly False_Press release_975827</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_356611</t>
+  </si>
+  <si>
     <t>Politifact_FALSE_Press release_663386</t>
   </si>
   <si>
+    <t>Politifact_Mostly False_Press release_776948</t>
+  </si>
+  <si>
     <t>Politifact_Mostly False_Press release_398964</t>
   </si>
   <si>
-    <t>Politifact_Mostly False_Press release_975827</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_712587</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_776948</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_356611</t>
+    <t>MADISON - In the early weeks of the COVID-19 crisis, unemployment in Wisconsin quickly
+began to skyrocket. Despite an overwhelming plea from Wisconsin residents to eliminate the
+one-week waiting period for unemployment, Senator Patrick Testin (R-Stevens Point) along with
+his fellow Rebublican colleagues waited for over a month to act. Their failure to quickly
+eliminate this bureaucratic red tape that they initially put in place has resulted in Wisconsin
+losing out on $25 million in federal funds for unemployment benefits.
+“I can think of $25 million reasons why Senator Testin shouldn’t be re-elected to the State
+Senate,” said SSDC Executive Director Eric LaGesse. “It is unfathomable that he would refuse
+to do his job when it means helping Wisconsin workers and families that are being hit the hardest
+by COVID-19. Residents in the 24th Senate District deserve a legislator that is going to fight
+tooth and nail for them and Patrick Testin clearly isn’t that person.”</t>
   </si>
   <si>
     <t xml:space="preserve">HAZLETON, PA -  Yesterday, June 11, Matt Cartwright showed his true liberal colors. When asked if “we should quit wasting money” on Wilkes-Barre police and "move that money around" to causes, Cartwright answered unequivocally “absolutely yes!"
 Bognet for Congress released the following comment in response to Cartwright’s outrageous idea to “Defund the Police.”
 "Matt Cartwright’s proposal to defund law enforcement is a radical and dangerous idea, and shows once again that he would rather cater to the latest leftist fad than represent the interests of Northeast Pennsylvania," Bognet for Congress spokesman Charles Russell said.
 A poll recently released by ABC/Ipsos released Friday, June 12, showed 64% of voters oppose defunding the police. Matt Cartwright has failed to be a voice for his constituents, promoting the values of coastal elites instead of hard working Pennsylvanians. </t>
-  </si>
-  <si>
-    <t>MADISON, Wis. - Regardless of any election’s outcome, it is imperative that every citizen be confident in the
-honesty and integrity of what is inarguably one of our most valuable constitutional rights.
-A great number of irregularities have taken place leading up to and including this past Election Day that have breached the trust of the electorate and created an environment of no-confidence in the outcomes of the November 3rd election.
-The only way to restore that trust and confidence is to perform a complete and in-depth investigative audit of the election and to hold off on certifying the election results until the investigation is complete.
-“Democrats have created a cloud of suspicion over this election because they refuse to follow state election laws. Conducting such an investigation prior to certifying the election is essential and the only way our citizens will believe the results reported are legitimate,” Sanfelippo said.
-The WI Election Commission ignored state law and refused to deactivate the eligibility of more than 230,000 unverified names on the voter list. Clerks in Milwaukee and Dane Counties colluded to nearly 250,000 individuals to the “Indefinitely Confined” voter list. Officials in the City of Madison defied state law confirmed by a court ruling and began early voting weeks ahead of the time allowed by law. Third Party candidates were kept off the ballot to protect the “chosen party” candidates. This is just the beginning of the list.
-If an investigation shows these actions affected the outcome of the election, we need to either declare this past election null and void and hold a new election or require our Electoral College Delegates to correct the injustice with their votes.
-“If we do not take action now to enforce our election laws and restore confidence in the outcomes, we will create an environment wherein each side tries to “out-cheat” the other to get to victory and We the People will lose permanent control as we fall victim to a government created of, by, and for the party,” said Sanfelippo.</t>
-  </si>
-  <si>
-    <t>Madison--State Representative John Nygren (R-Marinette), Co-Chair of the Joint Committee on
-Finance released the following statement:
-“Governor Evers’ sudden concern for rural Wisconsin and our agriculture industry is ironic
-given that just a year ago he proposed raising taxes on the agriculture industry to pay for
-expanded welfare programs,” said Rep. Nygren. “Governor Evers spent his first year in office
-catering to his far-left liberal friends in Madison. No amount of rhetoric can cover his failed
-record of putting rural Wisconsin and our farmer behind liberal special interests.”
-“Unfortunately, Governor Evers spent his first year in office trying to undo all the positive
-momentum of the last eight years,” said Rep. Nygren. “Between the largest property tax increase
-in the last 10 years, attempts to put more Wisconsinites on welfare, and a blatant disregard for
-state law, the last year for Governor Evers has been unacceptable. Wisconsin needs Governor
-Evers to change course in year two.”
-“The state of the state is strong, not because of Governor Evers, but in spite of him,” said Rep.
-Nygren. “Republicans in the Legislature have spent the last year listening to families all across
-Wisconsin and advancing an agenda for all of Wisconsin, not just Madison and Milwaukee.
-Governor Evers needs to reverse course and begin listening to all of Wisconsin instead of only
-the liberal special interests.”</t>
   </si>
   <si>
     <t>JEFFERSON CITY — During today’s COVID-19 briefing, Governor Mike Parson announced the first phase of the “Show Me Strong Recovery” Plan outlining how Missouri will gradually begin to reopen economic and social activity on Monday, May 4, 2020. 
@@ -236,31 +226,6 @@
 Pictures from today’s briefing will be available on Governor Parson’s Flickr page.</t>
   </si>
   <si>
-    <t>MADISON - In the early weeks of the COVID-19 crisis, unemployment in Wisconsin quickly
-began to skyrocket. Despite an overwhelming plea from Wisconsin residents to eliminate the
-one-week waiting period for unemployment, Senator Patrick Testin (R-Stevens Point) along with
-his fellow Rebublican colleagues waited for over a month to act. Their failure to quickly
-eliminate this bureaucratic red tape that they initially put in place has resulted in Wisconsin
-losing out on $25 million in federal funds for unemployment benefits.
-“I can think of $25 million reasons why Senator Testin shouldn’t be re-elected to the State
-Senate,” said SSDC Executive Director Eric LaGesse. “It is unfathomable that he would refuse
-to do his job when it means helping Wisconsin workers and families that are being hit the hardest
-by COVID-19. Residents in the 24th Senate District deserve a legislator that is going to fight
-tooth and nail for them and Patrick Testin clearly isn’t that person.”</t>
-  </si>
-  <si>
-    <t>(WISCONSIN) — Trump’s failed COVID-19 response has crushed farmers in Wisconsin and across the country. Farmers have been dumping milk, setting their crops on fire, and euthanizing their livestock because there is no market for their products. All the while, millions of more Americans are going hungry because they lost their jobs.
-But farmers were struggling long before coronavirus hit the United States. Trump’s chaotic trade wars, particularly with China, obliterated the markets Wisconsin farmers spent decades building in just a short few months. During this time Trump and his administration told Wisconsinites the pain would be “temporary,” that farmers were “over the hump,” and that small and medium-sized family farms should just get bigger if they want to survive.
-Trump has never seen farmers as more than a political pawn critical to his reelection chances. He used their pain to push through a multi-billion dollar bailout program that was nothing more than a handout for large agricultural companies. After getting rolled by China on a trade deal that was a mere fraction of what he promised it would be, a recent news report confirms that Trump was never interested in bettering the lives of Wisconsin’s farmers and was simply looking out for his own political interests.
-“Donald Trump crushed our farmers and the local economies they support because he only sees them as a bargaining chip, not human beings and Wisconsinites,” Democratic Party of Wisconsin spokesperson Philip Shulman said. “Trump has been a lapdog for China as he has rolled over for them at every turn. It’s been made clear by recent news reports that Trump gambled with farmers’ livelihoods because he thought it would be good for his reelection prospects. But after decimating these communities, they’re not willing to give him another four years — they know they can’t afford it.”
-Wisconsin Examiner: Farms go from frying pan of trade wars to fire of COVID-19
-Coxhead said trade policies under President Donald Trump…contributed significantly to the plight of Wisconsin farmers in the last few years. The federal government’s management of the COVID-19 pandemic has further endangered the country’s — and Wisconsin’s — position in the world economy, he added.
-Wisconsin State Farmer: Economic recovery after pandemic will be slow for farmers due to trade and internet issues
-He also said the Trump administration’s volatile relationship with China, one of the country’s biggest trading partners, is a cause for concern. And a widespread lack of high-speed internet access in rural areas is causing many rural economies to fall behind entirely. “The global economic recovery, which will outpace the United States, is not really going to benefit us all that well because the administration has turned its back on international trade,” Coxhead said.
-Milwaukee Journal Sentinel: Coronavirus has hit Wisconsin dairy farms especially hard — some farmers may even have to dump milk
-Coronavirus is delivering a blow to Wisconsin agriculture…export markets are threatened by global trade unrest, and some farms may not make it through the spring. “The coronavirus outbreak has caused milk prices to drop down to unprofitable levels this spring…We also need to be prepared for the scenarios that would require our members to dump milk”…”or dispose of (it) in some other manner,”…the stimulus package won’t resolve long-term issues such as increased global competition and trade wars that may arise from countries closing their borders to curb the spread of COVID-19. The global pandemic has sent a shock wave throughout agriculture.</t>
-  </si>
-  <si>
     <t>DREAM Act applications roll in while Excelsior Scholarship applications are suspended by One Party Rule in New York
 ALBANY, NY – The New York State Senate Republican Conference today slammed Democrats who have kept applications granting free tuition to illegal immigrants open while closing the Excelsior Scholarship application available to citizen students, whose families are struggling even more due to forced business closures during the coronavirus pandemic.
 “Time and time again, Democrats show New Yorkers their true priorities and under One Party Rule, illegal immigrants come before hardworking, law-abiding New Yorkers. When Senate Democrats voted to create free tuition for illegal immigrants, Republicans said no. To add insult to injury, so many families are facing an even more dire financial hardship after Governor Cuomo forced their livelihoods shut. To close citizen students out of the application process while continuing to give illegal immigrants free tuition is ludicrous. New Yorkers shouldn’t be funding tuition for illegal immigrants at all, and we should be closing down that program permanently as we look to find savings in our budget,” said Senate Republican Leader Rob Ortt.
@@ -276,42 +241,79 @@
 “It is unconscionable that Democrats would punish students whose only crime is that they are citizens.  It is no wonder that hard-working New York families are leaving the state in droves,” said Senator Andrew Lanza.</t>
   </si>
   <si>
+    <t>MADISON, Wis. - Regardless of any election’s outcome, it is imperative that every citizen be confident in the
+honesty and integrity of what is inarguably one of our most valuable constitutional rights.
+A great number of irregularities have taken place leading up to and including this past Election Day that have breached the trust of the electorate and created an environment of no-confidence in the outcomes of the November 3rd election.
+The only way to restore that trust and confidence is to perform a complete and in-depth investigative audit of the election and to hold off on certifying the election results until the investigation is complete.
+“Democrats have created a cloud of suspicion over this election because they refuse to follow state election laws. Conducting such an investigation prior to certifying the election is essential and the only way our citizens will believe the results reported are legitimate,” Sanfelippo said.
+The WI Election Commission ignored state law and refused to deactivate the eligibility of more than 230,000 unverified names on the voter list. Clerks in Milwaukee and Dane Counties colluded to nearly 250,000 individuals to the “Indefinitely Confined” voter list. Officials in the City of Madison defied state law confirmed by a court ruling and began early voting weeks ahead of the time allowed by law. Third Party candidates were kept off the ballot to protect the “chosen party” candidates. This is just the beginning of the list.
+If an investigation shows these actions affected the outcome of the election, we need to either declare this past election null and void and hold a new election or require our Electoral College Delegates to correct the injustice with their votes.
+“If we do not take action now to enforce our election laws and restore confidence in the outcomes, we will create an environment wherein each side tries to “out-cheat” the other to get to victory and We the People will lose permanent control as we fall victim to a government created of, by, and for the party,” said Sanfelippo.</t>
+  </si>
+  <si>
+    <t>(WISCONSIN) — Trump’s failed COVID-19 response has crushed farmers in Wisconsin and across the country. Farmers have been dumping milk, setting their crops on fire, and euthanizing their livestock because there is no market for their products. All the while, millions of more Americans are going hungry because they lost their jobs.
+But farmers were struggling long before coronavirus hit the United States. Trump’s chaotic trade wars, particularly with China, obliterated the markets Wisconsin farmers spent decades building in just a short few months. During this time Trump and his administration told Wisconsinites the pain would be “temporary,” that farmers were “over the hump,” and that small and medium-sized family farms should just get bigger if they want to survive.
+Trump has never seen farmers as more than a political pawn critical to his reelection chances. He used their pain to push through a multi-billion dollar bailout program that was nothing more than a handout for large agricultural companies. After getting rolled by China on a trade deal that was a mere fraction of what he promised it would be, a recent news report confirms that Trump was never interested in bettering the lives of Wisconsin’s farmers and was simply looking out for his own political interests.
+“Donald Trump crushed our farmers and the local economies they support because he only sees them as a bargaining chip, not human beings and Wisconsinites,” Democratic Party of Wisconsin spokesperson Philip Shulman said. “Trump has been a lapdog for China as he has rolled over for them at every turn. It’s been made clear by recent news reports that Trump gambled with farmers’ livelihoods because he thought it would be good for his reelection prospects. But after decimating these communities, they’re not willing to give him another four years — they know they can’t afford it.”
+Wisconsin Examiner: Farms go from frying pan of trade wars to fire of COVID-19
+Coxhead said trade policies under President Donald Trump…contributed significantly to the plight of Wisconsin farmers in the last few years. The federal government’s management of the COVID-19 pandemic has further endangered the country’s — and Wisconsin’s — position in the world economy, he added.
+Wisconsin State Farmer: Economic recovery after pandemic will be slow for farmers due to trade and internet issues
+He also said the Trump administration’s volatile relationship with China, one of the country’s biggest trading partners, is a cause for concern. And a widespread lack of high-speed internet access in rural areas is causing many rural economies to fall behind entirely. “The global economic recovery, which will outpace the United States, is not really going to benefit us all that well because the administration has turned its back on international trade,” Coxhead said.
+Milwaukee Journal Sentinel: Coronavirus has hit Wisconsin dairy farms especially hard — some farmers may even have to dump milk
+Coronavirus is delivering a blow to Wisconsin agriculture…export markets are threatened by global trade unrest, and some farms may not make it through the spring. “The coronavirus outbreak has caused milk prices to drop down to unprofitable levels this spring…We also need to be prepared for the scenarios that would require our members to dump milk”…”or dispose of (it) in some other manner,”…the stimulus package won’t resolve long-term issues such as increased global competition and trade wars that may arise from countries closing their borders to curb the spread of COVID-19. The global pandemic has sent a shock wave throughout agriculture.</t>
+  </si>
+  <si>
+    <t>Madison--State Representative John Nygren (R-Marinette), Co-Chair of the Joint Committee on
+Finance released the following statement:
+“Governor Evers’ sudden concern for rural Wisconsin and our agriculture industry is ironic
+given that just a year ago he proposed raising taxes on the agriculture industry to pay for
+expanded welfare programs,” said Rep. Nygren. “Governor Evers spent his first year in office
+catering to his far-left liberal friends in Madison. No amount of rhetoric can cover his failed
+record of putting rural Wisconsin and our farmer behind liberal special interests.”
+“Unfortunately, Governor Evers spent his first year in office trying to undo all the positive
+momentum of the last eight years,” said Rep. Nygren. “Between the largest property tax increase
+in the last 10 years, attempts to put more Wisconsinites on welfare, and a blatant disregard for
+state law, the last year for Governor Evers has been unacceptable. Wisconsin needs Governor
+Evers to change course in year two.”
+“The state of the state is strong, not because of Governor Evers, but in spite of him,” said Rep.
+Nygren. “Republicans in the Legislature have spent the last year listening to families all across
+Wisconsin and advancing an agenda for all of Wisconsin, not just Madison and Milwaukee.
+Governor Evers needs to reverse course and begin listening to all of Wisconsin instead of only
+the liberal special interests.”</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_839651</t>
+  </si>
+  <si>
+    <t>Politifact_FALSE_Press release_361429</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_697408</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_606127</t>
+  </si>
+  <si>
     <t>Politifact_FALSE_Press release_522440</t>
   </si>
   <si>
-    <t>Politifact_FALSE_Press release_361429</t>
+    <t>Politifact_Mostly False_Press release_151890</t>
+  </si>
+  <si>
+    <t>Politifact_FALSE_Press release_179292</t>
   </si>
   <si>
     <t>Politifact_FALSE_Press release_645229</t>
   </si>
   <si>
+    <t>Politifact_Mostly False_Press release_88472</t>
+  </si>
+  <si>
     <t>Politifact_FALSE_Press release_890060</t>
   </si>
   <si>
-    <t>Politifact_FALSE_Press release_179292</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_88472</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_839651</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_151890</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_606127</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_697408</t>
-  </si>
-  <si>
-    <t>Today, Congressman Glenn Grothman (WI-06) released the following statement after the House adopted rules to eliminate, among others, the words “Mother”, “Father”, “Son”, and “Daughter”.
-“One of the first actions taken by the Democrat-controlled House of Representatives was to eliminate the words father, mother, son, daughter, brother, sister, uncle, aunt, first cousin, nephew, niece, husband, wife, father-in-law, mother-in-law, son-in-law, daughter-in-law, brother-in-law, sister-in-law, stepfather, stepmother, stepson, stepdaughter, stepbrother, stepsister, half brother, half sister, grandson, and granddaughter,” said Grothman. “Up to this point, the plot to eradicate the traditional family has been reserved for the fringe left-wing. But now, a majority of Americans have voted for a party that wants to fundamentally change our country and wants a world in which you cannot call your parents mom and dad. I don’t think this represents the true feelings of most Americans and if they knew they sent representatives to Washington who have blacklisted the words ‘mother’ and ‘father’, they would be appalled.
-“While I have many friends in the Democratic party, we cannot pretend that there are not men and women in the world and that everybody is the same. People must begin to realize that the America that has provided opportunities to millions, regardless of their race, gender, or orientation, is disappearing before our eyes.
-“While this decision is largely symbolic, it is now the official position of the U.S. House of Representatives that these words are offensive and shall not be used. I will not dishonor my mother and father and all of the effort they put into raising two sons and two daughters by removing these words from my vocabulary.”
--30-
-U.S. Rep. Glenn Grothman is serving his fourth term representing Wisconsin’s 6th Congressional District in the U.S. House of Representatives.</t>
+    <t xml:space="preserve">WASHINGTON, DC – U.S. Congressman Scott Fitzgerald (WI-05) made the following statement after voting against the Democrats’ $1.9 trillion pandemic “relief” proposal that spends less than 9% on COVID-19 related measures: 
+“To say this budget proposal is irresponsible would be an understatement of the century. More than 91% of the spending in this $1.9 trillion package is not used for pandemic relief. In fact, some of the funding is being funneled into pet projects like Senator Schumer’s bridge and Speaker Pelosi’s tunnel. The Democrats’ continue to show just how out of touch they are with everyday Americans. Students need schools to reopen; small businesses need to stay open; and workers need the opportunity to go to work. Unlike the CARES Act, which delivered legitimate relief, this bill does little to address the current and immediate needs of Wisconsinites.” </t>
   </si>
   <si>
     <t>STATE OF FLORIDA
@@ -347,13 +349,28 @@
 Continue reading the full Executive Order here.</t>
   </si>
   <si>
-    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released a weekly update on his actions to address America’s debt crisis and rising inflation. As the wasteful, reckless spending of the Biden administration and congressional Democrats leads to growing inflation and rising prices of every day goods, Senator Scott is urging the president to end his failed economic policies and address rising inflation on American families.
-This week, Senator Rick Scott spoke on the Senate floor on how Democrats’ reckless tax-and-spending spree is causing rising inflation and hurting American families. Senator Scott also led several of his colleagues in a press conference today on how Congress can work to get government spending under control, including passing his Federal Debt Emergency Control Act to require that two-thirds of the Senate vote to increase the debt before approving any bill with deficit spending, and his amendment to the Senate Rules to require that all committee reports include inflationary impact statements so Americans can see the true impacts of government spending.
-Senator Rick Scott said, “Biden and the Democrats say they care about Americans – but they have done absolutely nothing to help families struggling to keep up with inflation. We are nearly $30 TRILLION in debt, but Democrats have no plans to slow down their spending. Now, Biden and the Democrats want to spend another $5.5 trillion on their liberal priorities, with no consideration to how this might impact families. Their message to the American people is clear: they don’t care about inflation. They don’t care that their reckless spending is causing prices to skyrocket. If that’s the cost of getting their liberal wish list, so be it. It’s time to wake up and take action to get government spending under control – our children and grandchildren are depending on it.”
-See more in the video HERE or below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"The way Democrats talk about spending trillions of dollars like pocket change, while asking for a blank check book to spend as much as they want without worrying about the repercussions, should concern every single American. It is critical that we don’t default on our debts, but equally as important that we don’t allow Democrats to spend as much as they want, on whatever they want. We shouldn’t give Democrats a free pass to spend Iowans' money irresponsibly and jeopardize the entire global economy. Democrats should drop their multi-trillion-dollar social spending extravaganza and commit to working with Republicans to put our nation on a sustainable fiscal path that respects taxpayers." - Congresswoman Ashley Hinson </t>
+    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released the below statement slamming Biden’s inaction to address the inflation crisis he and Washington Democrats have created with reckless spending and socialist policies, which is expected to cause significant price increases on seniors citizens and Medicare recipients. According to a report from the Centers for Medicare &amp; Medicaid Services (CMS), Medicare Part B premiums and deductibles will both increase by 15% and Medicare Part A deductibles will increase by 5% in 2022, leaving seniors paying hundreds more for the health care and benefits they desperately need.
+Senator Rick Scott said, “Here’s my question for Joe Biden and Democrats: who is your reckless spending and socialist agenda helping? It’s clearly not families on fixed incomes, like mine growing up, struggling to keep up with inflation and put food on the table with higher and higher costs. It’s definitely not our businesses facing higher costs and a supply chain crisis fueled by Biden’s failed policies and unconstitutional vaccine mandates. And it’s obviously NOT our seniors depending on Medicare who will be left paying HUNDREDS more for the care they need. We need to be LOWERING health care and drug prices and strengthening this vital program for seniors and future generations, not crippling the system and leaving families to pay the cost. It’s now clearer than ever that Democrats don’t care who pays the price for their liberal wish list, they have their blinders on, following Bernie Sanders’ socialist lead on an all-or-nothing multi trillion dollar tax-and-spending spree. I came to Washington to FIGHT for our seniors. We cannot allow this to move forward.”</t>
+  </si>
+  <si>
+    <t>MADISON - Recently, Dr. Rochelle Walensky, the director of the Centers for Disease Control (CDC), stated that she wants the agency to establish gun violence as an urgent public health crisis. This would be a major step forward for gun safety as the CDC has largely been silent on gun violence research since 1997 due to a lack of Congressional funding. Senator Melissa Agard (D-Madison) released the following statement on this new commitment to address gun violence:
+“Gun violence is an urgent public health crisis. I am encouraged to see the CDC acknowledging the stark reality of too many lives lost each day. The fact is, no other country on the planet witnesses the number of gun deaths that we do here in the United States, and it’s not even close.
+“As Dr. Walensky said, this isn’t about restricting the rights of responsible gun owners. It’s about doing research to understand the full scope of the gun violence crisis in our country and identifying ways to address it.”</t>
+  </si>
+  <si>
+    <t>Today, Congressman Glenn Grothman (WI-06) released the following statement after the House adopted rules to eliminate, among others, the words “Mother”, “Father”, “Son”, and “Daughter”.
+“One of the first actions taken by the Democrat-controlled House of Representatives was to eliminate the words father, mother, son, daughter, brother, sister, uncle, aunt, first cousin, nephew, niece, husband, wife, father-in-law, mother-in-law, son-in-law, daughter-in-law, brother-in-law, sister-in-law, stepfather, stepmother, stepson, stepdaughter, stepbrother, stepsister, half brother, half sister, grandson, and granddaughter,” said Grothman. “Up to this point, the plot to eradicate the traditional family has been reserved for the fringe left-wing. But now, a majority of Americans have voted for a party that wants to fundamentally change our country and wants a world in which you cannot call your parents mom and dad. I don’t think this represents the true feelings of most Americans and if they knew they sent representatives to Washington who have blacklisted the words ‘mother’ and ‘father’, they would be appalled.
+“While I have many friends in the Democratic party, we cannot pretend that there are not men and women in the world and that everybody is the same. People must begin to realize that the America that has provided opportunities to millions, regardless of their race, gender, or orientation, is disappearing before our eyes.
+“While this decision is largely symbolic, it is now the official position of the U.S. House of Representatives that these words are offensive and shall not be used. I will not dishonor my mother and father and all of the effort they put into raising two sons and two daughters by removing these words from my vocabulary.”
+-30-
+U.S. Rep. Glenn Grothman is serving his fourth term representing Wisconsin’s 6th Congressional District in the U.S. House of Representatives.</t>
+  </si>
+  <si>
+    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released the third and fourth episode of Road Trip on a Budget, his video short series in partnership with The Heritage Foundation. Episode 3 highlights how Washington’s reckless spending is causing rising inflation, which means the prices of every day goods are going up for families in Florida and across the nation. Episode 4 discusses how Congress can work to rein in wasteful spending and why we must fight Democrats’ tax-and-spending spree agenda to put America back on a strong fiscal path. See previous Road Trip on a Budget episodes HERE and HERE.
+Senator Rick Scott said, “Reckless government spending has driven America’s federal debt to nearly $30 trillion. Now, thanks to the insane tax-and-spending spree of President Joe Biden and Democrats in Washington, we are seeing six straight months of raging inflation. It’s time to face reality, ditch these foolish and wasteful multi-trillion dollar plans and protect American families from rising inflation. With the debt ceiling suspension expiring this week, on July 31, we need real spending reform, like my Federal Debt Emergency Control Act, before we consider raising the debt ceiling. We cannot allow Congress to continue mortgaging the futures of our children and grandchildren.” 
+Matthew Dickerson, director of Heritage’s Hermann Center for the Federal Budget, said, “The importance of Congress exercising spending restraint instead of continuing down the path of seemingly endless, reckless federal spending cannot be understated. For instance, Democrats are looking to pass a $3.5 trillion budget kickstarting the reconciliation process to pass all of their legislative priorities, including non-budget related policies like mass amnesty, and few are talking about the consequences. This budget resolution represents more of the same fiscal irresponsibility. When the federal government grows beyond its proper limits, and spends and taxes too much, it stifles prosperity, infringes on liberty, and makes it more difficult to live the American dream. Thanks to Sen. Rick Scott’s leadership, more Americans will be able to learn about the dangers of big-government spending adding recklessly to the national debt and increasing inflation, and by extension, prices of good Americans buy every day.”
+Watch the third episode HERE or below.
+Watch the fourth episode HERE or below.</t>
   </si>
   <si>
     <t xml:space="preserve">Business and Economic Neighborhood Development
@@ -373,55 +390,43 @@
 Chicago hit an all time venture capital funding record, with $7.9 billion in 2021 alone, a figure that puts it just behind the long-standing top-tier tech hubs of San Francisco, New York, Boston, and Los Angeles in terms of venture capital investment. The total was more than $1 billion more than Chicago startups raised in all of 2020, representing a stunning funding trajectory. </t>
   </si>
   <si>
+    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released a weekly update on his actions to address America’s debt crisis and rising inflation. As the wasteful, reckless spending of the Biden administration and congressional Democrats leads to growing inflation and rising prices of every day goods, Senator Scott is urging the president to end his failed economic policies and address rising inflation on American families.
+This week, Senator Rick Scott spoke on the Senate floor on how Democrats’ reckless tax-and-spending spree is causing rising inflation and hurting American families. Senator Scott also led several of his colleagues in a press conference today on how Congress can work to get government spending under control, including passing his Federal Debt Emergency Control Act to require that two-thirds of the Senate vote to increase the debt before approving any bill with deficit spending, and his amendment to the Senate Rules to require that all committee reports include inflationary impact statements so Americans can see the true impacts of government spending.
+Senator Rick Scott said, “Biden and the Democrats say they care about Americans – but they have done absolutely nothing to help families struggling to keep up with inflation. We are nearly $30 TRILLION in debt, but Democrats have no plans to slow down their spending. Now, Biden and the Democrats want to spend another $5.5 trillion on their liberal priorities, with no consideration to how this might impact families. Their message to the American people is clear: they don’t care about inflation. They don’t care that their reckless spending is causing prices to skyrocket. If that’s the cost of getting their liberal wish list, so be it. It’s time to wake up and take action to get government spending under control – our children and grandchildren are depending on it.”
+See more in the video HERE or below.</t>
+  </si>
+  <si>
     <t>WASHINGTON, D.C. – Today, Senator Rick Scott released the below statement about Democrats’ plans to use the $1.9 trillion COVID-19 spending package to bailout wasteful states, like New York, Illinois and California, that want to use taxpayer money to backfill their poorly-managed budgets and pension plans.
 Senator Rick Scott said, “Senate Republicans are all in for getting targeted relief to Americans that are still hurting from this pandemic. But President Biden and the Democrats want to spend more than $350 billion to bailout their friends in New York, Illinois, and California. And they are lying about the need for this money. Congress has already given states roughly $400 billion to combat this crisis. States across the country are seeing increases in revenue — in some cases, well above projections. Now, we are learning that 47 states show an average decline of just 0.12 percent compared to 2019, and twenty-one of the 47 states show positive year over year growth of tax receipts. Over half of states reported positive growth, including California, New York, and Illinois.
 “This is great news for our states – but Democrats don’t want you to know this. The Democrats have made it blatantly obvious that this isn’t about helping people – it’s a payback to their friends for helping with their campaigns. Less than two weeks into the Biden Administration and Democrats have already completely abandoned their inauthentic calls for ‘unity’ and ‘bipartisanship’ just to push through massive spending and get tax dollars to their buddies. You can’t make this stuff up. These wasteful states just have their hand out to the federal government in hopes that American taxpayers will plug the long-standing holes in their budgets and pension systems created by decades of mismanagement and the poor decisions of failed politicians. That’s not fair to Floridians and all the states around the country that have been working hard to protect taxpayer dollars. We can’t let it happen.”
 See more in Senator Scott’s interview with FOX News yesterday .</t>
   </si>
   <si>
-    <t xml:space="preserve">WASHINGTON, DC – U.S. Congressman Scott Fitzgerald (WI-05) made the following statement after voting against the Democrats’ $1.9 trillion pandemic “relief” proposal that spends less than 9% on COVID-19 related measures: 
-“To say this budget proposal is irresponsible would be an understatement of the century. More than 91% of the spending in this $1.9 trillion package is not used for pandemic relief. In fact, some of the funding is being funneled into pet projects like Senator Schumer’s bridge and Speaker Pelosi’s tunnel. The Democrats’ continue to show just how out of touch they are with everyday Americans. Students need schools to reopen; small businesses need to stay open; and workers need the opportunity to go to work. Unlike the CARES Act, which delivered legitimate relief, this bill does little to address the current and immediate needs of Wisconsinites.” </t>
-  </si>
-  <si>
-    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released the third and fourth episode of Road Trip on a Budget, his video short series in partnership with The Heritage Foundation. Episode 3 highlights how Washington’s reckless spending is causing rising inflation, which means the prices of every day goods are going up for families in Florida and across the nation. Episode 4 discusses how Congress can work to rein in wasteful spending and why we must fight Democrats’ tax-and-spending spree agenda to put America back on a strong fiscal path. See previous Road Trip on a Budget episodes HERE and HERE.
-Senator Rick Scott said, “Reckless government spending has driven America’s federal debt to nearly $30 trillion. Now, thanks to the insane tax-and-spending spree of President Joe Biden and Democrats in Washington, we are seeing six straight months of raging inflation. It’s time to face reality, ditch these foolish and wasteful multi-trillion dollar plans and protect American families from rising inflation. With the debt ceiling suspension expiring this week, on July 31, we need real spending reform, like my Federal Debt Emergency Control Act, before we consider raising the debt ceiling. We cannot allow Congress to continue mortgaging the futures of our children and grandchildren.” 
-Matthew Dickerson, director of Heritage’s Hermann Center for the Federal Budget, said, “The importance of Congress exercising spending restraint instead of continuing down the path of seemingly endless, reckless federal spending cannot be understated. For instance, Democrats are looking to pass a $3.5 trillion budget kickstarting the reconciliation process to pass all of their legislative priorities, including non-budget related policies like mass amnesty, and few are talking about the consequences. This budget resolution represents more of the same fiscal irresponsibility. When the federal government grows beyond its proper limits, and spends and taxes too much, it stifles prosperity, infringes on liberty, and makes it more difficult to live the American dream. Thanks to Sen. Rick Scott’s leadership, more Americans will be able to learn about the dangers of big-government spending adding recklessly to the national debt and increasing inflation, and by extension, prices of good Americans buy every day.”
-Watch the third episode HERE or below.
-Watch the fourth episode HERE or below.</t>
-  </si>
-  <si>
-    <t>MADISON - Recently, Dr. Rochelle Walensky, the director of the Centers for Disease Control (CDC), stated that she wants the agency to establish gun violence as an urgent public health crisis. This would be a major step forward for gun safety as the CDC has largely been silent on gun violence research since 1997 due to a lack of Congressional funding. Senator Melissa Agard (D-Madison) released the following statement on this new commitment to address gun violence:
-“Gun violence is an urgent public health crisis. I am encouraged to see the CDC acknowledging the stark reality of too many lives lost each day. The fact is, no other country on the planet witnesses the number of gun deaths that we do here in the United States, and it’s not even close.
-“As Dr. Walensky said, this isn’t about restricting the rights of responsible gun owners. It’s about doing research to understand the full scope of the gun violence crisis in our country and identifying ways to address it.”</t>
-  </si>
-  <si>
-    <t>WASHINGTON, D.C. – Today, Senator Rick Scott released the below statement slamming Biden’s inaction to address the inflation crisis he and Washington Democrats have created with reckless spending and socialist policies, which is expected to cause significant price increases on seniors citizens and Medicare recipients. According to a report from the Centers for Medicare &amp; Medicaid Services (CMS), Medicare Part B premiums and deductibles will both increase by 15% and Medicare Part A deductibles will increase by 5% in 2022, leaving seniors paying hundreds more for the health care and benefits they desperately need.
-Senator Rick Scott said, “Here’s my question for Joe Biden and Democrats: who is your reckless spending and socialist agenda helping? It’s clearly not families on fixed incomes, like mine growing up, struggling to keep up with inflation and put food on the table with higher and higher costs. It’s definitely not our businesses facing higher costs and a supply chain crisis fueled by Biden’s failed policies and unconstitutional vaccine mandates. And it’s obviously NOT our seniors depending on Medicare who will be left paying HUNDREDS more for the care they need. We need to be LOWERING health care and drug prices and strengthening this vital program for seniors and future generations, not crippling the system and leaving families to pay the cost. It’s now clearer than ever that Democrats don’t care who pays the price for their liberal wish list, they have their blinders on, following Bernie Sanders’ socialist lead on an all-or-nothing multi trillion dollar tax-and-spending spree. I came to Washington to FIGHT for our seniors. We cannot allow this to move forward.”</t>
+    <t xml:space="preserve">"The way Democrats talk about spending trillions of dollars like pocket change, while asking for a blank check book to spend as much as they want without worrying about the repercussions, should concern every single American. It is critical that we don’t default on our debts, but equally as important that we don’t allow Democrats to spend as much as they want, on whatever they want. We shouldn’t give Democrats a free pass to spend Iowans' money irresponsibly and jeopardize the entire global economy. Democrats should drop their multi-trillion-dollar social spending extravaganza and commit to working with Republicans to put our nation on a sustainable fiscal path that respects taxpayers." - Congresswoman Ashley Hinson </t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_752020</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_954534</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_746218</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_296819</t>
+  </si>
+  <si>
+    <t>Politifact_Mostly False_Press release_587828</t>
   </si>
   <si>
     <t>Politifact_FALSE_Press release_691928</t>
   </si>
   <si>
-    <t>Politifact_Mostly False_Press release_954534</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_746218</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_752020</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_587828</t>
-  </si>
-  <si>
-    <t>Politifact_Mostly False_Press release_296819</t>
-  </si>
-  <si>
-    <t>Richmond, VA – As the special session begins today, it is clear that Governor Youngkin’s incompetence continues to harm Virginians, with most glaring example being his failure to secure an agreement on the budget despite holding the majority in the House. Now, through his failed leadership, crucial funds localities rely on to function are at risk. This comes after Governor Youngkin called legislators back to Richmond through a privately funded campaign ad – taking some members of his own party by surprise – while still refusing to agree to key funding issues for our public schools and health care infrastructure in our communities. 
-Senate Democrats this session proposed a comprehensive budget that will invest in Virginia’s public schools, support hard-working teachers and prepare students for good-paying jobs of the future in the energy, health, and education sectors. They will continue to push for smart tax cuts for everyday Virginians in addition to essential community investments. The future of the Commonwealth’s economy depends on strong health, wellness and education infrastructure, as well as access to opportunity for each and every resident.
-This session, Republicans launched attack after attack on Virginia’s public schools, teachers and students. They have repeatedly threatened to defund public education and their budget is proof of their true intentions. The proposed House budget cuts hundreds of millions in funding for public education, including gutting teacher pay raises by 20% and slashing tens of millions in funding for early childhood education.
-The budget proposed by House Republicans also includes millions of cuts to successful and proven programs like the Virginia Mental Health Access Project, which provides critical care to young people and slashed more than $10 million in funding for permanent supportive housing, a program that provides housing and wraparound services, allowing individuals experiencing mental illness to live in community-based settings.
-““It is embarrassing and unprecedented for a Governor who has the majority in the House to still not have an agreement on the budget after calling legislators back to Richmond  – a move that cost taxpayers $40,000,” said DPVA Chairwoman Susan Swecker. “Governor Youngkin’s failure to pass a budget and support important investments in our childrens’ futures and our health care infrastructure is now hurting local governments and Virginians. His incompetent leadership is a danger to our Commonwealth and I am thankful that Virginia Democrats are fighting for generational investments in our futures and ensuring the longevity of our Commonwealth.”</t>
+    <t>OSHKOSH – On Thursday, U.S. Sen. Ron Johnson (R-Wis.), member of the Senate Homeland Security and Governmental Affairs Committee, and U.S. Sen. Rob Portman (R-Ohio), Ranking Member of the Senate Homeland Security and Governmental Affairs Committee, introduced legislation to prohibit the Administrator of the Transportation Security Administration (TSA) from accepting arrest warrants as valid proof of identification at airport security checkpoints and for other purposes. The senators introduced this legislation after TSA confirmed its use of arrest warrants, issued by Immigrations and Customs Enforcement (ICE), to help confirm the identity of unlawful migrants for travel by air.
+“I am happy to introduce legislation that will aid in securing our border and help stop President Biden’s disastrous open border policies. The Biden administration’s disregard for the rule of law knows no bounds. Since the president took office a year ago, we have seen at least 2.4 million people enter this country illegally. For DHS and TSA to allow known criminals who possess an arrest warrant to fly on U.S. aircraft threatens our homeland security. This out-of-control flow of illegal immigration that has created the crisis at the border is a direct result of the Biden administration’s policies,” said Johnson.
+“It is concerning that DHS and TSA are allowing individuals to fly on U.S. aircraft based on unverified personal data provided to CBP or ICE when these people crossed the border unlawfully. This policy is a national security threat and should be revoked as quickly as possible. It is policies like these from the Biden administration that give the green light to human smugglers and drug traffickers that they can unlawfully enter our country. This administration must change course and instill policies that help secure our border. That’s why I’ve introduced this legislation to prohibit the TSA from accepting arrest warrants of unlawful migrants as valid proof of identification,” said Portman.
+The full text of the bill can be found here.</t>
   </si>
   <si>
     <t>What we witnessed yesterday was the last gasps of a corrupt and discredited left-wing political and media establishment that has, for decades, driven our country into the ground—shipping away our jobs, surrendering our strength, sacrificing our sovereignty, attacking our history and values, and trying to turn America into a country that our people can barely recognize.
@@ -445,10 +450,17 @@
 "It shouldn't surprise Iowans that Finkenauer doesn't know what's in the bill even though she supports it. She is saying the quiet part out loud - she will be a rubber stamp for Joe Biden's agenda," said Republican Party of Iowa Communications Director Kollin Crompton. "Iowans deserve to know if Bohannan and Mathis stand with their party's leaders on this disastrous legislation."</t>
   </si>
   <si>
-    <t>OSHKOSH – On Thursday, U.S. Sen. Ron Johnson (R-Wis.), member of the Senate Homeland Security and Governmental Affairs Committee, and U.S. Sen. Rob Portman (R-Ohio), Ranking Member of the Senate Homeland Security and Governmental Affairs Committee, introduced legislation to prohibit the Administrator of the Transportation Security Administration (TSA) from accepting arrest warrants as valid proof of identification at airport security checkpoints and for other purposes. The senators introduced this legislation after TSA confirmed its use of arrest warrants, issued by Immigrations and Customs Enforcement (ICE), to help confirm the identity of unlawful migrants for travel by air.
-“I am happy to introduce legislation that will aid in securing our border and help stop President Biden’s disastrous open border policies. The Biden administration’s disregard for the rule of law knows no bounds. Since the president took office a year ago, we have seen at least 2.4 million people enter this country illegally. For DHS and TSA to allow known criminals who possess an arrest warrant to fly on U.S. aircraft threatens our homeland security. This out-of-control flow of illegal immigration that has created the crisis at the border is a direct result of the Biden administration’s policies,” said Johnson.
-“It is concerning that DHS and TSA are allowing individuals to fly on U.S. aircraft based on unverified personal data provided to CBP or ICE when these people crossed the border unlawfully. This policy is a national security threat and should be revoked as quickly as possible. It is policies like these from the Biden administration that give the green light to human smugglers and drug traffickers that they can unlawfully enter our country. This administration must change course and instill policies that help secure our border. That’s why I’ve introduced this legislation to prohibit the TSA from accepting arrest warrants of unlawful migrants as valid proof of identification,” said Portman.
-The full text of the bill can be found here.</t>
+    <t>MADISON — In a year when students across the nation experienced declines, Wisconsin elementary school students held steady in mathematics and reading assessment scores released today by the National Assessment of Educational Progress (NAEP), also known as the “Nation’s Report Card.” Consistent with national trends, Wisconsin eighth grade students experienced declines in both subjects, but overall scores remained at or above the national average.
+“The results released today reiterate trends we have seen across the nation as students continue to recover from learning disruptions caused by the COVID-19 pandemic,” State Superintendent Dr. Jill Underly said. “Recovery is a continuous journey, and we haven’t yet reached a destination we are satisfied with, nor do we just want to return to where we were before. What is clear is that Wisconsin students, educators, and schools need our support more than ever. They are our future, and we owe it to them to invest in their success and ensure they are well prepared to lead this state.”
+The 2022 NAEP results are the first glimpse at how the COVID-19 pandemic may have affected students academically on the national level. NAEP is the largest nationally representative and continuing assessment of what the nation’s students know and can do in various subject areas.
+In mathematics, Wisconsin was one of 10 states/jurisdictions without any significant statistical change among fourth graders from 2019, with students performing above the national average scale score. In the same subject, the state’s eighth graders were among 51 states/jurisdictions experiencing score declines from 2019, though Wisconsin eighth graders remain above the national average. In reading, Wisconsin fourth graders were among 22 states/jurisdictions that did not experience a significant statistical change from 2019. Wisconsin eighth graders were among 33 states/jurisdictions experiencing a decline in reading scores from 2019.
+NAEP results also showed the Black to white opportunity gap among Wisconsin fourth and eighth graders persists in both mathematics and reading. Wisconsin’s opportunity gap between Black and white students remains the widest among all states/jurisdictions, except the District of Columbia, according to NAEP results.
+“We’ve known Wisconsin’s racial disparities in assessment results are among the widest in the nation for too long, and these troubling results are yet one more indication that we must close the opportunity gap in our state,” Dr. Underly said. “We need continued investment, intervention, and innovation in our state, and we have the means to accomplish exactly that. Our biennial budget request will help put targeted resources and supports in our schools and ensure we are helping the students who need it the most at this critical time. They deserve no less, and neither do we.”
+The 2022 NAEP was taken by students from January to March 2022 and was previously taken by students in early 2019. The national assessment is typically administered on a two-year basis. About 2,200 Wisconsin fourth graders and about 2,600 eighth graders were tested in reading. About 2,300 Wisconsin fourth graders and about 2,500 eighth graders were tested in mathematics.
+Wisconsin’s full state report can be found on the NAEP website, along with the national report. For more information on NAEP in Wisconsin, visit the Wisconsin Department of Public Instruction’s website.
+Results for NAEP’s Trial Urban District Assessment were also released today with state results. Milwaukee Public Schools is among 26 large urban school districts that participate in TUDA. More information and results for TUDAs can be found on the NAEP’s website.
+Official Release
+dpinr2022-61.pdf</t>
   </si>
   <si>
     <t>The organized effort to rescue the children of Communist Cuba 50 years ago is a far cry from the Biden administration’s disgraceful border disaster
@@ -469,17 +481,11 @@
 Announcing proposals for the current Legislative Session to hold accountable private entities that knowingly or recklessly assist the Biden Administration in resettling illegal immigrants into Florida.</t>
   </si>
   <si>
-    <t>MADISON — In a year when students across the nation experienced declines, Wisconsin elementary school students held steady in mathematics and reading assessment scores released today by the National Assessment of Educational Progress (NAEP), also known as the “Nation’s Report Card.” Consistent with national trends, Wisconsin eighth grade students experienced declines in both subjects, but overall scores remained at or above the national average.
-“The results released today reiterate trends we have seen across the nation as students continue to recover from learning disruptions caused by the COVID-19 pandemic,” State Superintendent Dr. Jill Underly said. “Recovery is a continuous journey, and we haven’t yet reached a destination we are satisfied with, nor do we just want to return to where we were before. What is clear is that Wisconsin students, educators, and schools need our support more than ever. They are our future, and we owe it to them to invest in their success and ensure they are well prepared to lead this state.”
-The 2022 NAEP results are the first glimpse at how the COVID-19 pandemic may have affected students academically on the national level. NAEP is the largest nationally representative and continuing assessment of what the nation’s students know and can do in various subject areas.
-In mathematics, Wisconsin was one of 10 states/jurisdictions without any significant statistical change among fourth graders from 2019, with students performing above the national average scale score. In the same subject, the state’s eighth graders were among 51 states/jurisdictions experiencing score declines from 2019, though Wisconsin eighth graders remain above the national average. In reading, Wisconsin fourth graders were among 22 states/jurisdictions that did not experience a significant statistical change from 2019. Wisconsin eighth graders were among 33 states/jurisdictions experiencing a decline in reading scores from 2019.
-NAEP results also showed the Black to white opportunity gap among Wisconsin fourth and eighth graders persists in both mathematics and reading. Wisconsin’s opportunity gap between Black and white students remains the widest among all states/jurisdictions, except the District of Columbia, according to NAEP results.
-“We’ve known Wisconsin’s racial disparities in assessment results are among the widest in the nation for too long, and these troubling results are yet one more indication that we must close the opportunity gap in our state,” Dr. Underly said. “We need continued investment, intervention, and innovation in our state, and we have the means to accomplish exactly that. Our biennial budget request will help put targeted resources and supports in our schools and ensure we are helping the students who need it the most at this critical time. They deserve no less, and neither do we.”
-The 2022 NAEP was taken by students from January to March 2022 and was previously taken by students in early 2019. The national assessment is typically administered on a two-year basis. About 2,200 Wisconsin fourth graders and about 2,600 eighth graders were tested in reading. About 2,300 Wisconsin fourth graders and about 2,500 eighth graders were tested in mathematics.
-Wisconsin’s full state report can be found on the NAEP website, along with the national report. For more information on NAEP in Wisconsin, visit the Wisconsin Department of Public Instruction’s website.
-Results for NAEP’s Trial Urban District Assessment were also released today with state results. Milwaukee Public Schools is among 26 large urban school districts that participate in TUDA. More information and results for TUDAs can be found on the NAEP’s website.
-Official Release
-dpinr2022-61.pdf</t>
+    <t>Richmond, VA – As the special session begins today, it is clear that Governor Youngkin’s incompetence continues to harm Virginians, with most glaring example being his failure to secure an agreement on the budget despite holding the majority in the House. Now, through his failed leadership, crucial funds localities rely on to function are at risk. This comes after Governor Youngkin called legislators back to Richmond through a privately funded campaign ad – taking some members of his own party by surprise – while still refusing to agree to key funding issues for our public schools and health care infrastructure in our communities. 
+Senate Democrats this session proposed a comprehensive budget that will invest in Virginia’s public schools, support hard-working teachers and prepare students for good-paying jobs of the future in the energy, health, and education sectors. They will continue to push for smart tax cuts for everyday Virginians in addition to essential community investments. The future of the Commonwealth’s economy depends on strong health, wellness and education infrastructure, as well as access to opportunity for each and every resident.
+This session, Republicans launched attack after attack on Virginia’s public schools, teachers and students. They have repeatedly threatened to defund public education and their budget is proof of their true intentions. The proposed House budget cuts hundreds of millions in funding for public education, including gutting teacher pay raises by 20% and slashing tens of millions in funding for early childhood education.
+The budget proposed by House Republicans also includes millions of cuts to successful and proven programs like the Virginia Mental Health Access Project, which provides critical care to young people and slashed more than $10 million in funding for permanent supportive housing, a program that provides housing and wraparound services, allowing individuals experiencing mental illness to live in community-based settings.
+““It is embarrassing and unprecedented for a Governor who has the majority in the House to still not have an agreement on the budget after calling legislators back to Richmond  – a move that cost taxpayers $40,000,” said DPVA Chairwoman Susan Swecker. “Governor Youngkin’s failure to pass a budget and support important investments in our childrens’ futures and our health care infrastructure is now hurting local governments and Virginians. His incompetent leadership is a danger to our Commonwealth and I am thankful that Virginia Democrats are fighting for generational investments in our futures and ensuring the longevity of our Commonwealth.”</t>
   </si>
   <si>
     <t>Politifact_Mostly False_Press release_453309</t>
@@ -494,13 +500,19 @@
 “As Ron DeSantis once again leaves Floridians behind to advance his own political ambitions, DeSantis Watch is proud to help introduce his out-of-touch and extreme record to a wider audience,” said DeSantis Watch Communications Director Anders Croy. “There is no greater threat to our freedoms than Ron DeSantis, a fake populist whose subservience to billionaires and the corporate elites will mean higher costs for you, cuts to Medicare and a shorter retirement with your family, and weakness in the face of Putin’s aggression in Ukraine. That’s Ron DeSantis’ real blueprint for America.”</t>
   </si>
   <si>
+    <t>Politifact_FALSE_Press release_315880</t>
+  </si>
+  <si>
     <t>Politifact_FALSE_Press release_814222</t>
   </si>
   <si>
-    <t>Politifact_FALSE_Press release_315880</t>
-  </si>
-  <si>
     <t>Politifact_Mostly False_Press release_648457</t>
+  </si>
+  <si>
+    <t>The Justice System in New York State, and America as a whole, is under assault by partisan, deluded, biased Judges and Prosecutors. Racist, Corrupt A.G. Tish James has been obsessed with “Getting Trump” for years, and used Crooked New York State Judge Engoron to get an illegal, unAmerican judgment against me, my family, and my tremendous business. I helped New York City during its worst of times, and now, while it is overrun with Violent Biden Migrant Crime, the Radicals are doing all they can to kick me out.
+This “decision” is a Complete and Total SHAM. There were No Victims, No Damages, No Complaints. Only satisfied Banks and Insurance Companies (which made a ton of money), GREAT Financial Statements, that didn’t even include the most valuable Asset - The TRUMP Brand, IRONCLAD Disclaimers (Buyer Beware, and Do your Own Due Diligence), and amazing Properties all over the World. All the other side had was a ridiculous $18 million valuation of magnificent Mar-a-Lago, an unConstitutional Gag Order, a Consumer Fraud Statute never before used for this purpose, No Jury allowed, and a refusal to send this disgusting charade to the Commercial Division, where it would have been put to a deserving end.
+This “case” is OVER ever since the Appellate Division ended it on Statute of Limitations, also letting my daughter Ivanka out of this Witch Hunt. The Democrat Club-controlled Judge Engoron has already been reversed four times on this case, a shameful record, and he will be reversed again. We cannot let injustice stand, and will fight Crooked Joe Biden’s weaponized persecution at every step. MAKE AMERICA GREAT AGAIN!
+Read the Truths here, here, and here.</t>
   </si>
   <si>
     <t xml:space="preserve">WASHINGTON, D.C. – Senators Thom Tillis (R-NC) and Marsha Blackburn (R-TN) recently introduced the Safe and Open Streets Act, legislation that would make it a federal crime to purposely obstruct, delay, or affect commerce by blocking a public road or highway. 
@@ -509,12 +521,6 @@
 “The emerging tactic of radical protestors blocking roads and stopping commerce is not only obnoxious to innocent commuters, but it’s also dangerous and will eventually get people killed. It needs to be a crime throughout the country,” said Senator Tillis. “I’m proud to introduce the Safe and Open Streets Act so radical activists who resort to these reckless and dangerous tactics are held accountable under the full weight of the law for endangering public safety.” 
 “Blocking major roads to stop traffic flows is nothing short of lawlessness that should not be tolerated,” said Senator Blackburn. “These activists are not only intentionally creating a dangerous situation for themselves, but perhaps for a citizen who is awaiting an ambulance or a hard worker who will lose their job for being late. The Safe and Open Streets Act is critical to stopping this reckless behavior, particularly by Hamas sympathizers, in our U.S. cities.”
 The text of the Safe and Open Streets Act can be found here. </t>
-  </si>
-  <si>
-    <t>The Justice System in New York State, and America as a whole, is under assault by partisan, deluded, biased Judges and Prosecutors. Racist, Corrupt A.G. Tish James has been obsessed with “Getting Trump” for years, and used Crooked New York State Judge Engoron to get an illegal, unAmerican judgment against me, my family, and my tremendous business. I helped New York City during its worst of times, and now, while it is overrun with Violent Biden Migrant Crime, the Radicals are doing all they can to kick me out.
-This “decision” is a Complete and Total SHAM. There were No Victims, No Damages, No Complaints. Only satisfied Banks and Insurance Companies (which made a ton of money), GREAT Financial Statements, that didn’t even include the most valuable Asset - The TRUMP Brand, IRONCLAD Disclaimers (Buyer Beware, and Do your Own Due Diligence), and amazing Properties all over the World. All the other side had was a ridiculous $18 million valuation of magnificent Mar-a-Lago, an unConstitutional Gag Order, a Consumer Fraud Statute never before used for this purpose, No Jury allowed, and a refusal to send this disgusting charade to the Commercial Division, where it would have been put to a deserving end.
-This “case” is OVER ever since the Appellate Division ended it on Statute of Limitations, also letting my daughter Ivanka out of this Witch Hunt. The Democrat Club-controlled Judge Engoron has already been reversed four times on this case, a shameful record, and he will be reversed again. We cannot let injustice stand, and will fight Crooked Joe Biden’s weaponized persecution at every step. MAKE AMERICA GREAT AGAIN!
-Read the Truths here, here, and here.</t>
   </si>
   <si>
     <t>The Biden Administration and Senator Baldwin have fueled the worst border crisis in our nation’s history. Their refusal to secure our southern border and enforce our immigration laws has put the security of our nation at great risk, allowed the unabated flow of drugs from Mexico and China, and created a humanitarian crisis for migrants.
@@ -905,13 +911,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,49 +927,64 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.03702928870292887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.03431372549019608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.02331288343558282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>4817</v>
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.01876675603217158</v>
       </c>
     </row>
   </sheetData>
@@ -973,13 +994,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,82 +1010,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.0392156862745098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.0303030303030303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.01692524682651622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.01131221719457014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>0.008928571428571428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0.008756567425569177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>879</v>
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>0.004464285714285714</v>
       </c>
     </row>
   </sheetData>
@@ -1074,13 +1119,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,115 +1135,148 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.04615384615384616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.04605263157894737</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.03731343283582089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.03636363636363636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>0.02333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0.01630434782608696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>0.01354401805869074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>0.01324503311258278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="C2">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>0.0124223602484472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="C3">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
       <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11">
-        <v>269</v>
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1208,13 +1286,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1224,71 +1302,92 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.06050955414012739</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.02724358974358974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.02654867256637168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.02527075812274368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="C2">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>0.01009174311926606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="C3">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
       <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7">
-        <v>571</v>
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0.007537688442211055</v>
       </c>
     </row>
   </sheetData>
@@ -1298,13 +1397,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,16 +1413,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2">
-        <v>331</v>
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.00303951367781155</v>
       </c>
     </row>
   </sheetData>
@@ -1333,13 +1438,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,38 +1454,50 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.039568345323741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="C2">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
       <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.026578073089701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="C3">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4">
-        <v>327</v>
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.00308641975308642</v>
       </c>
     </row>
   </sheetData>
@@ -1398,31 +1515,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1433,25 +1550,25 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1558</v>
+        <v>0.02835566341521984</v>
       </c>
       <c r="D2">
-        <v>2188.543046564693</v>
+        <v>0.008719844303743063</v>
       </c>
       <c r="E2">
-        <v>211</v>
+        <v>0.01876675603217158</v>
       </c>
       <c r="F2">
-        <v>331.75</v>
+        <v>0.02217635158473001</v>
       </c>
       <c r="G2">
-        <v>602</v>
+        <v>0.02881330446288945</v>
       </c>
       <c r="H2">
-        <v>1828.25</v>
+        <v>0.03499261629337928</v>
       </c>
       <c r="I2">
-        <v>4817</v>
+        <v>0.03702928870292887</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1462,25 +1579,25 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>431.5714285714286</v>
+        <v>0.01712937216672182</v>
       </c>
       <c r="D3">
-        <v>293.7424365794276</v>
+        <v>0.01286463437434025</v>
       </c>
       <c r="E3">
-        <v>134</v>
+        <v>0.004464285714285714</v>
       </c>
       <c r="F3">
-        <v>190</v>
+        <v>0.008842569427070303</v>
       </c>
       <c r="G3">
-        <v>338</v>
+        <v>0.01131221719457014</v>
       </c>
       <c r="H3">
-        <v>645</v>
+        <v>0.02361413856477326</v>
       </c>
       <c r="I3">
-        <v>879</v>
+        <v>0.0392156862745098</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1491,25 +1608,25 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>338.1</v>
+        <v>0.02447326395113918</v>
       </c>
       <c r="D4">
-        <v>237.1761886118512</v>
+        <v>0.01598500960777592</v>
       </c>
       <c r="E4">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>193.25</v>
+        <v>0.01331977934910977</v>
       </c>
       <c r="G4">
-        <v>298</v>
+        <v>0.01981884057971015</v>
       </c>
       <c r="H4">
-        <v>358.5</v>
+        <v>0.03707598371777476</v>
       </c>
       <c r="I4">
-        <v>942</v>
+        <v>0.04615384615384616</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1520,25 +1637,25 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>520</v>
+        <v>0.02620033435571827</v>
       </c>
       <c r="D5">
-        <v>335.5878424496335</v>
+        <v>0.01890490655685544</v>
       </c>
       <c r="E5">
-        <v>115</v>
+        <v>0.007537688442211055</v>
       </c>
       <c r="F5">
-        <v>339.75</v>
+        <v>0.01388649687013546</v>
       </c>
       <c r="G5">
-        <v>486.5</v>
+        <v>0.02590971534455768</v>
       </c>
       <c r="H5">
-        <v>604.75</v>
+        <v>0.02706986044928523</v>
       </c>
       <c r="I5">
-        <v>1097</v>
+        <v>0.06050955414012739</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1549,22 +1666,22 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
       <c r="E6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
       <c r="F6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
       <c r="G6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
       <c r="H6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
       <c r="I6">
-        <v>331</v>
+        <v>0.00303951367781155</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1575,25 +1692,25 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>301.6666666666667</v>
+        <v>0.02307761272217614</v>
       </c>
       <c r="D7">
-        <v>25.00666577801474</v>
+        <v>0.01849115032722828</v>
       </c>
       <c r="E7">
-        <v>277</v>
+        <v>0.00308641975308642</v>
       </c>
       <c r="F7">
-        <v>289</v>
+        <v>0.01483224642139371</v>
       </c>
       <c r="G7">
-        <v>301</v>
+        <v>0.026578073089701</v>
       </c>
       <c r="H7">
-        <v>314</v>
+        <v>0.033073209206721</v>
       </c>
       <c r="I7">
-        <v>327</v>
+        <v>0.039568345323741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>